<commit_message>
Updated BOM to provide technique for soldering the MAX 10 FPGA
</commit_message>
<xml_diff>
--- a/Kicad/ElectronULA - MAX 10 Board V1.02/BOM.xlsx
+++ b/Kicad/ElectronULA - MAX 10 Board V1.02/BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ElectronULA" localSheetId="0">Sheet1!$A$14:$I$31</definedName>
+    <definedName name="ElectronULA" localSheetId="0">Sheet1!$A$15:$I$32</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -282,13 +282,7 @@
     <t>Tips</t>
   </si>
   <si>
-    <t>3. All the passives (capacitors, resistors), comparator and regulator etc are best done with solder flux and a hot air gun. I would avoid doing this to the SW1 switch however as it may melt it. The switch is best done with the soldering iron</t>
-  </si>
-  <si>
     <t>Excellent drag soldering guide here "https://www.youtube.com/watch?v=nyele3CIs-U"</t>
-  </si>
-  <si>
-    <t>2. I recommend using a gel like flux for the SMD chips. Run plenty along each row of pads and then align the chip correctly, the gel helps keep the chip in place. Tag each corner by soldering one or two pins and then drag solder the rest. See guide below</t>
   </si>
   <si>
     <t>https://www.ebay.co.uk/i/292483310138?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=710-134428-41853-0&amp;mkcid=2&amp;itemid=292483310138&amp;targetid=908661474856&amp;device=c&amp;mktype=pla&amp;googleloc=9046613&amp;poi=&amp;campaignid=10195651586&amp;mkgroupid=107296210212&amp;rlsatarget=pla-908661474856&amp;abcId=1145987&amp;merchantid=7398364&amp;gclid=EAIaIQobChMI6ru5t-WQ6gIVzoKyCh1oBwxIEAQYCiABEgImJvD_BwE</t>
@@ -311,6 +305,15 @@
       </rPr>
       <t>Check on your socket before doing this though just in case</t>
     </r>
+  </si>
+  <si>
+    <t>3. I recommend using a gel like flux for the SMD chips. Run plenty along each row of pads and then align the chip correctly, the gel helps keep the chip in place. Tag each corner by soldering one or two pins and then drag solder the rest. See guide below</t>
+  </si>
+  <si>
+    <t>4. All the passives (capacitors, resistors), comparator and regulator etc are best done with solder flux and a hot air gun. I would avoid doing this to the SW1 switch however as it may melt it. The switch is best done with the soldering iron</t>
+  </si>
+  <si>
+    <t>2. Soldering the MAX 10 FPGA - Place a small amount of solder paste on the large central pad and then place the chip accordingly with gel flux applied to the pads as per point 3. Drag solder the pins first and then heat the chip from the other side of the board with a hot air gun to hopefully melt the solder paste. I'm not sure this is the correct technique but thats the process I used.</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -785,13 +788,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" s="16"/>
     </row>
@@ -807,440 +810,446 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="9"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <v>2</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D17" s="3">
         <v>1</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>3</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D18" s="3">
         <v>19</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>4</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
+        <v>7</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="3">
+        <v>26</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>8</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>9</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>11</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="3">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
+        <v>12</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>13</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D28" s="3">
         <v>1</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G28" s="14" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>14</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="3">
-        <v>6</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D29" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>62</v>
+        <v>35</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
+        <v>15</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>16</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>17</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>17</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="15"/>
     </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="15"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G15" r:id="rId1"/>
-    <hyperlink ref="G18" r:id="rId2"/>
-    <hyperlink ref="G28" r:id="rId3"/>
-    <hyperlink ref="G30" r:id="rId4"/>
-    <hyperlink ref="G24" r:id="rId5" display="https://www.digikey.co.uk/product-detail/en/diodes-incorporated/AP2114H-3.3TRG1/AP2114H-3.3TRG1DICT-ND/4505142?utm_adgroup=PMIC%20-%20Voltage%20Regulators%20-%20Linear&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Google%20Shopping_Integrated%20Circuits%20%28ICs%29&amp;utm_term=&amp;productid=4505142&amp;gclid=EAIaIQobChMIkoq-teuO6gIVC4myCh0O7wooEAQYASABEgJpyfD_BwE"/>
-    <hyperlink ref="G27" r:id="rId6"/>
-    <hyperlink ref="G29" r:id="rId7"/>
-    <hyperlink ref="G16" r:id="rId8"/>
+    <hyperlink ref="G16" r:id="rId1"/>
+    <hyperlink ref="G19" r:id="rId2"/>
+    <hyperlink ref="G29" r:id="rId3"/>
+    <hyperlink ref="G31" r:id="rId4"/>
+    <hyperlink ref="G25" r:id="rId5" display="https://www.digikey.co.uk/product-detail/en/diodes-incorporated/AP2114H-3.3TRG1/AP2114H-3.3TRG1DICT-ND/4505142?utm_adgroup=PMIC%20-%20Voltage%20Regulators%20-%20Linear&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Google%20Shopping_Integrated%20Circuits%20%28ICs%29&amp;utm_term=&amp;productid=4505142&amp;gclid=EAIaIQobChMIkoq-teuO6gIVC4myCh0O7wooEAQYASABEgJpyfD_BwE"/>
+    <hyperlink ref="G28" r:id="rId6"/>
+    <hyperlink ref="G30" r:id="rId7"/>
+    <hyperlink ref="G17" r:id="rId8"/>
     <hyperlink ref="A5" r:id="rId9" display="https://www.ebay.co.uk/i/292483310138?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=710-134428-41853-0&amp;mkcid=2&amp;itemid=292483310138&amp;targetid=908661474856&amp;device=c&amp;mktype=pla&amp;googleloc=9046613&amp;poi=&amp;campaignid=10195651586&amp;mkgroupid=107296210212&amp;rlsatarget=pla-908661474856&amp;abcId=1145987&amp;merchantid=7398364&amp;gclid=EAIaIQobChMI6ru5t-WQ6gIVzoKyCh1oBwxIEAQYCiABEgImJvD_BwE"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>